<commit_message>
Remove ID3 from the code
</commit_message>
<xml_diff>
--- a/FilteredDB.xlsx
+++ b/FilteredDB.xlsx
@@ -898,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
@@ -2227,7 +2227,7 @@
         <v>7800</v>
       </c>
       <c r="O24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P24" t="n">
         <v>0</v>
@@ -2896,7 +2896,7 @@
         <v>0</v>
       </c>
       <c r="P33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q33" t="n">
         <v>0</v>
@@ -3041,7 +3041,7 @@
         <v>8182.442748091603</v>
       </c>
       <c r="O35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P35" t="n">
         <v>0</v>
@@ -4447,7 +4447,7 @@
         <v>7100</v>
       </c>
       <c r="O54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P54" t="n">
         <v>1</v>
@@ -4595,7 +4595,7 @@
         <v>9400</v>
       </c>
       <c r="O56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P56" t="n">
         <v>1</v>
@@ -5483,7 +5483,7 @@
         <v>10700</v>
       </c>
       <c r="O68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P68" t="n">
         <v>0</v>
@@ -6001,7 +6001,7 @@
         <v>9000</v>
       </c>
       <c r="O75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P75" t="n">
         <v>1</v>
@@ -7037,7 +7037,7 @@
         <v>8182.442748091603</v>
       </c>
       <c r="O89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P89" t="n">
         <v>0</v>
@@ -8591,7 +8591,7 @@
         <v>12800</v>
       </c>
       <c r="O110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P110" t="n">
         <v>1</v>
@@ -8739,7 +8739,7 @@
         <v>4200</v>
       </c>
       <c r="O112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P112" t="n">
         <v>1</v>
@@ -9257,7 +9257,7 @@
         <v>5800</v>
       </c>
       <c r="O119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P119" t="n">
         <v>0</v>
@@ -9997,7 +9997,7 @@
         <v>7900</v>
       </c>
       <c r="O129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P129" t="n">
         <v>1</v>
@@ -11921,7 +11921,7 @@
         <v>9800</v>
       </c>
       <c r="O155" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P155" t="n">
         <v>0</v>

</xml_diff>